<commit_message>
Update Docs Support Team Project Management.xlsx
</commit_message>
<xml_diff>
--- a/Docs Support Team Project Management.xlsx
+++ b/Docs Support Team Project Management.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\01_Projects\04_MS Project Management\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Qinglin\Documents\GitHub\Project01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{984FCFFF-47DF-4535-866E-1D007E1DD4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7DA2FF-D591-4180-B176-AE6E67B52A18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>User Story</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>Learn the Help Documents and prepare a doc publishing workshop</t>
+  </si>
+  <si>
+    <t>In Progress</t>
   </si>
 </sst>
 </file>
@@ -408,7 +411,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,6 +449,9 @@
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
       <c r="E2" t="s">
         <v>9</v>
       </c>

</xml_diff>